<commit_message>
rMATS must have more than 2 samples for each group
</commit_message>
<xml_diff>
--- a/snakemake/meta/contrast.as.xlsx
+++ b/snakemake/meta/contrast.as.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T5/Dropbox (UMass Medical School)/projects/OneStopRNAseq/OneStopRNAseq_mac/snakemake/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A2AB92-767A-6F4A-B70C-91953C0EFABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667A679C-E7E1-C840-A3F6-AA01ADF1AAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="6080" windowWidth="27620" windowHeight="18160" xr2:uid="{B12AF396-C96E-44D7-9EB8-1B46E0EECA2A}"/>
+    <workbookView xWindow="16440" yWindow="5980" windowWidth="27620" windowHeight="18160" xr2:uid="{B12AF396-C96E-44D7-9EB8-1B46E0EECA2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>KO_D0</t>
   </si>
@@ -470,215 +470,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7195E0-7987-4741-8EEA-5CA7C29AB060}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="246" zoomScaleNormal="246" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>